<commit_message>
add a list for multiple files
</commit_message>
<xml_diff>
--- a/files/PIST_HER.xlsx
+++ b/files/PIST_HER.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F111"/>
+  <dimension ref="A1:F103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,16 +477,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4974.06</v>
+        <v>5968.7</v>
       </c>
       <c r="D2" t="n">
-        <v>467.64</v>
+        <v>338.44</v>
       </c>
       <c r="E2" t="n">
-        <v>51.61</v>
+        <v>158.95</v>
       </c>
       <c r="F2" t="n">
-        <v>5493.31</v>
+        <v>6466.089999999999</v>
       </c>
     </row>
     <row r="3">
@@ -501,16 +501,16 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>9321.49</v>
+        <v>8420.58</v>
       </c>
       <c r="D3" t="n">
-        <v>276.85</v>
+        <v>299.25</v>
       </c>
       <c r="E3" t="n">
-        <v>14.2</v>
+        <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>9612.540000000001</v>
+        <v>8719.83</v>
       </c>
     </row>
     <row r="4">
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>5199.01</v>
+        <v>5351.03</v>
       </c>
       <c r="D4" t="n">
-        <v>245.41</v>
+        <v>227.1</v>
       </c>
       <c r="E4" t="n">
-        <v>-32.16</v>
+        <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>5412.26</v>
+        <v>5578.13</v>
       </c>
     </row>
     <row r="5">
@@ -549,16 +549,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>18051.93</v>
+        <v>14075.88</v>
       </c>
       <c r="D5" t="n">
-        <v>512.24</v>
+        <v>354.44</v>
       </c>
       <c r="E5" t="n">
-        <v>113.48</v>
+        <v>134.31</v>
       </c>
       <c r="F5" t="n">
-        <v>18677.65</v>
+        <v>14564.63</v>
       </c>
     </row>
     <row r="6">
@@ -573,16 +573,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>9914.219999999999</v>
+        <v>3445.69</v>
       </c>
       <c r="D6" t="n">
-        <v>-188.91</v>
+        <v>263.86</v>
       </c>
       <c r="E6" t="n">
         <v>15.64</v>
       </c>
       <c r="F6" t="n">
-        <v>9740.949999999999</v>
+        <v>3725.19</v>
       </c>
     </row>
     <row r="7">
@@ -600,13 +600,13 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>-50.85</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>-50.85</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -621,304 +621,304 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17310.16</v>
+        <v>11715</v>
       </c>
       <c r="D8" t="n">
-        <v>-68.09</v>
+        <v>324.5</v>
       </c>
       <c r="E8" t="n">
-        <v>131.65</v>
+        <v>116.23</v>
       </c>
       <c r="F8" t="n">
-        <v>17373.72</v>
+        <v>12155.73</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>0052</t>
+          <t>0056</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ΒΛΑΧΟΣ ΒΑΣΙΛΕΙΟΣ</t>
+          <t>ΒΑΡΔΙΑΜΠΑΣΗΣ ΚΩΝΣΤΑΝΤΙΝΟΣ</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>4693.6</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>243</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>12.8</v>
+        <v>273.6</v>
       </c>
       <c r="F9" t="n">
-        <v>4949.400000000001</v>
+        <v>273.6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>0188</t>
+          <t>0052</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ΒΟΛΩΝΑΚΗΣ ΑΧΙΛΛΕΑΣ</t>
+          <t>ΒΛΑΧΟΣ ΒΑΣΙΛΕΙΟΣ</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>19144.59</v>
+        <v>4660.37</v>
       </c>
       <c r="D10" t="n">
-        <v>152.56</v>
+        <v>206.38</v>
       </c>
       <c r="E10" t="n">
-        <v>627.55</v>
+        <v>77.47</v>
       </c>
       <c r="F10" t="n">
-        <v>19924.7</v>
+        <v>4944.22</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>0610</t>
+          <t>0188</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ΒΡΕΝΤΖΟΣ ΙΩΑΝΝΗΣ</t>
+          <t>ΒΟΛΩΝΑΚΗΣ ΑΧΙΛΛΕΑΣ</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>20690.45</v>
+        <v>21219.18</v>
       </c>
       <c r="D11" t="n">
-        <v>-318.73</v>
+        <v>312.49</v>
       </c>
       <c r="E11" t="n">
-        <v>44.01</v>
+        <v>242.08</v>
       </c>
       <c r="F11" t="n">
-        <v>20415.73</v>
+        <v>21773.75</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>0080</t>
+          <t>0610</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>ΓΟΥΡΝΙΕΖΑΚΗΣ ΜΑΤΘΑΙΟΣ</t>
+          <t>ΒΡΕΝΤΖΟΣ ΙΩΑΝΝΗΣ</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>23464.82</v>
+        <v>14321.64</v>
       </c>
       <c r="D12" t="n">
-        <v>1074.37</v>
+        <v>116.86</v>
       </c>
       <c r="E12" t="n">
-        <v>160.93</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>24700.12</v>
+        <v>14438.5</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>0999</t>
+          <t>0080</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ΔΑΚΑΝΑΛΗ ΑΝΑΣΤΑΣΙΑ</t>
+          <t>ΓΟΥΡΝΙΕΖΑΚΗΣ ΜΑΤΘΑΙΟΣ</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>15501.54</v>
+        <v>16627.42</v>
       </c>
       <c r="D13" t="n">
-        <v>291.9</v>
+        <v>916.4</v>
       </c>
       <c r="E13" t="n">
-        <v>25.5</v>
+        <v>187.86</v>
       </c>
       <c r="F13" t="n">
-        <v>15818.94</v>
+        <v>17731.68</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>0085</t>
+          <t>0999</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ΔΑΝΕΛΑΚΗΣ ΚΩΝΣΤΑΝΤΙΝΟΣ</t>
+          <t>ΔΑΚΑΝΑΛΗ ΑΝΑΣΤΑΣΙΑ</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>4258.53</v>
+        <v>13793.29</v>
       </c>
       <c r="D14" t="n">
-        <v>-151.57</v>
+        <v>303.78</v>
       </c>
       <c r="E14" t="n">
-        <v>0</v>
+        <v>39.6</v>
       </c>
       <c r="F14" t="n">
-        <v>4106.96</v>
+        <v>14136.67</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>0057</t>
+          <t>0085</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ΔΑΣΚΑΛΑΚΗ ΑΙΚΑΤΕΡΙΝΗ(ΡΕΘΥΜΝΟ)</t>
+          <t>ΔΑΝΕΛΑΚΗΣ ΚΩΝΣΤΑΝΤΙΝΟΣ</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>3753.2</v>
       </c>
       <c r="D15" t="n">
-        <v>93</v>
+        <v>108.72</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>93</v>
+        <v>3861.92</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>0106</t>
+          <t>0057</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>ΔΙΑΚΑΚΗ-ΚΟΚΚΙΝΑΚΗ ΕΥΑΓ-ΚΟΚΚΙΝΑΚΗ ΜΑΡΙΝΑ ΣΦ ΟΕ</t>
+          <t>ΔΑΣΚΑΛΑΚΗ ΑΙΚΑΤΕΡΙΝΗ(ΡΕΘΥΜΝΟ)</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>14121.42</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>229.55</v>
+        <v>80.27</v>
       </c>
       <c r="E16" t="n">
-        <v>176.64</v>
+        <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>14527.61</v>
+        <v>80.27</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>0329</t>
+          <t>0106</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>ΔΡΑΜΙΤΙΝΟΥ ΓΕΩΡΓΙΑ</t>
+          <t>ΔΙΑΚΑΚΗ-ΚΟΚΚΙΝΑΚΗ ΕΥΑΓ-ΚΟΚΚΙΝΑΚΗ ΜΑΡΙΝΑ ΣΦ ΟΕ</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>6037.08</v>
       </c>
       <c r="D17" t="n">
-        <v>-56.21</v>
+        <v>245.58</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>160.66</v>
       </c>
       <c r="F17" t="n">
-        <v>-56.21</v>
+        <v>6443.32</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1117</t>
+          <t>0329</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ΔΡΑΜΟΥΝΤΑΝΗΣ Γ ΕΥΑΓΓΕΛΟΣ</t>
+          <t>ΔΡΑΜΙΤΙΝΟΥ ΓΕΩΡΓΙΑ</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>14125.48</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>125.99</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>65.34</v>
+        <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>14316.81</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>0120</t>
+          <t>1117</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>ΖΑΧΑΡΕΝΑΚΗΣ ΙΩΑΝΝΗΣ</t>
+          <t>ΔΡΑΜΟΥΝΤΑΝΗΣ Γ ΕΥΑΓΓΕΛΟΣ</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>9969.040000000001</v>
+        <v>11295.81</v>
       </c>
       <c r="D19" t="n">
-        <v>399.66</v>
+        <v>182.11</v>
       </c>
       <c r="E19" t="n">
-        <v>0</v>
+        <v>55.99</v>
       </c>
       <c r="F19" t="n">
-        <v>10368.7</v>
+        <v>11533.91</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>0985</t>
+          <t>0120</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ΖΩΓΡΑΦΟΣ ΣΤΕΦΑΝΟΣ</t>
+          <t>ΖΑΧΑΡΕΝΑΚΗΣ ΙΩΑΝΝΗΣ</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>7956.3</v>
       </c>
       <c r="D20" t="n">
-        <v>-6.85</v>
+        <v>189.08</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>-6.85</v>
+        <v>8145.38</v>
       </c>
     </row>
     <row r="21">
@@ -936,13 +936,13 @@
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>-117.64</v>
+        <v>10.26</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
       </c>
       <c r="F21" t="n">
-        <v>-117.64</v>
+        <v>10.26</v>
       </c>
     </row>
     <row r="22">
@@ -960,2149 +960,1957 @@
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>-70.36</v>
+        <v>34.67</v>
       </c>
       <c r="E22" t="n">
         <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>-70.36</v>
+        <v>34.67</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>0805</t>
+          <t>0037</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>ΚΑΛΟΕΙΔΑ-ΒΑΡΔΙΑΜΠΑΣΗ ΕΛΕΝΗ</t>
+          <t>ΚΑΝΙΑΔΑΚΗΣ ΑΝΤΩΝΗΣ</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>700.38</v>
       </c>
       <c r="D23" t="n">
-        <v>28.98</v>
+        <v>410.15</v>
       </c>
       <c r="E23" t="n">
-        <v>0</v>
+        <v>58.26</v>
       </c>
       <c r="F23" t="n">
-        <v>28.98</v>
+        <v>1168.79</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>0037</t>
+          <t>0021</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>ΚΑΝΙΑΔΑΚΗΣ ΑΝΤΩΝΗΣ</t>
+          <t>ΚΑΡΟΥΖΑΚΗΣ ΕΥΑΓΓΕΛΟΣ &amp; ΣΙΑ ΕΕ</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>15241.43</v>
+        <v>5262.19</v>
       </c>
       <c r="D24" t="n">
-        <v>647.21</v>
+        <v>208.98</v>
       </c>
       <c r="E24" t="n">
-        <v>1184.7</v>
+        <v>46.08</v>
       </c>
       <c r="F24" t="n">
-        <v>17073.34</v>
+        <v>5517.249999999999</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>0021</t>
+          <t>0146</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>ΚΑΡΟΥΖΑΚΗΣ ΕΥΑΓΓΕΛΟΣ &amp; ΣΙΑ ΕΕ</t>
+          <t>ΚΑΤΑΛΑΓΑΡΙΑΝΟΥ Ι.ΕΥΑΓΓΕΛΙΑ</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>8055.22</v>
+        <v>3549.85</v>
       </c>
       <c r="D25" t="n">
-        <v>11.75</v>
+        <v>11.6</v>
       </c>
       <c r="E25" t="n">
-        <v>39.43</v>
+        <v>0</v>
       </c>
       <c r="F25" t="n">
-        <v>8106.400000000001</v>
+        <v>3561.45</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>0146</t>
+          <t>1068</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>ΚΑΤΑΛΑΓΑΡΙΑΝΟΥ Ι.ΕΥΑΓΓΕΛΙΑ</t>
+          <t>ΚΑΦΕΤΖΑΚΗ ΜΑΡΙΑ-ΤΖΩΡΑΚΟΛΕΥΘΕΡΑΚΗΣ ΒΑΣΙΛΕΙΟΣ ΜΑΡΙΟΣ ΣΦ ΟΕ</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>3450.97</v>
+        <v>11582.23</v>
       </c>
       <c r="D26" t="n">
-        <v>31.98</v>
+        <v>214.19</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>3.45</v>
       </c>
       <c r="F26" t="n">
-        <v>3482.95</v>
+        <v>11799.87</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>1068</t>
+          <t>0256</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>ΚΑΦΕΤΖΑΚΗ ΜΑΡΙΑ-ΤΖΩΡΑΚΟΛΕΥΘΕΡΑΚΗΣ ΒΑΣΙΛΕΙΟΣ ΜΑΡΙΟΣ ΣΦ ΟΕ</t>
+          <t>ΚΗΛΑΙΔΑΚΗΣ ΝΙΚΟΛΑΟΣ τ.ΗΛΙΑ</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>13604.62</v>
+        <v>6000.37</v>
       </c>
       <c r="D27" t="n">
-        <v>135.2</v>
+        <v>447.19</v>
       </c>
       <c r="E27" t="n">
-        <v>29.67</v>
+        <v>0</v>
       </c>
       <c r="F27" t="n">
-        <v>13769.49</v>
+        <v>6447.559999999999</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>0256</t>
+          <t>0169</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>ΚΗΛΑΙΔΑΚΗΣ ΝΙΚΟΛΑΟΣ τ.ΗΛΙΑ</t>
+          <t>ΚΛΑΨΙΝΑΚΗ ΜΑΡΙΑΝΝΑ</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>9559.040000000001</v>
+        <v>3596.15</v>
       </c>
       <c r="D28" t="n">
-        <v>443.81</v>
+        <v>42.36</v>
       </c>
       <c r="E28" t="n">
-        <v>9.970000000000001</v>
+        <v>0</v>
       </c>
       <c r="F28" t="n">
-        <v>10012.82</v>
+        <v>3638.51</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>0169</t>
+          <t>0170</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>ΚΛΑΨΙΝΑΚΗ ΜΑΡΙΑΝΝΑ</t>
+          <t>ΚΟΚΚΙΝΑΚΗΣ ΓΡΗΓΟΡΙΟΣ</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>4238.62</v>
+        <v>12195.1</v>
       </c>
       <c r="D29" t="n">
-        <v>30.16</v>
+        <v>292.17</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>180.13</v>
       </c>
       <c r="F29" t="n">
-        <v>4268.78</v>
+        <v>12667.4</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>0170</t>
+          <t>0341</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>ΚΟΚΚΙΝΑΚΗΣ ΓΡΗΓΟΡΙΟΣ</t>
+          <t>ΚΟΥΒΙΔΗ ΤΗΛ. ΕΥΑΓΓΕΛΙΑ</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>14654.17</v>
+        <v>17181.22</v>
       </c>
       <c r="D30" t="n">
-        <v>548.27</v>
+        <v>158.77</v>
       </c>
       <c r="E30" t="n">
-        <v>91.09</v>
+        <v>21.16</v>
       </c>
       <c r="F30" t="n">
-        <v>15293.53</v>
+        <v>17361.15</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>0341</t>
+          <t>0696</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>ΚΟΥΒΙΔΗ ΤΗΛ. ΕΥΑΓΓΕΛΙΑ</t>
+          <t>ΚΡΑΣΑΚΗΣ ΙΩΑΝΝΗΣ</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>23954.89</v>
+        <v>74.45</v>
       </c>
       <c r="D31" t="n">
-        <v>152.74</v>
+        <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>26.11</v>
+        <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>24133.74</v>
+        <v>74.45</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>0183</t>
+          <t>0243</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>ΚΟΥΤΕΝΤΑΚΗΣ ΔΗΜΗΤΡΙΟΣ</t>
+          <t>ΚΡΟΝΤΗΡΗΣ Δ. ΙΩΑΝΝΗΣ</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>3529.94</v>
+        <v>15643.69</v>
       </c>
       <c r="D32" t="n">
-        <v>83.53</v>
+        <v>612.78</v>
       </c>
       <c r="E32" t="n">
-        <v>176.25</v>
+        <v>776.48</v>
       </c>
       <c r="F32" t="n">
-        <v>3789.72</v>
+        <v>17032.95</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>0696</t>
+          <t>0195</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>ΚΡΑΣΑΚΗΣ ΙΩΑΝΝΗΣ</t>
+          <t>ΚΡΟΝΤΗΡΗΣ ΔΗΜΗΤΡΙΟΣ</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>33.9</v>
+        <v>7768.15</v>
       </c>
       <c r="D33" t="n">
-        <v>17.54</v>
+        <v>179.31</v>
       </c>
       <c r="E33" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F33" t="n">
-        <v>51.44</v>
+        <v>7977.46</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>0243</t>
+          <t>1173</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>ΚΡΟΝΤΗΡΗΣ Δ. ΙΩΑΝΝΗΣ</t>
+          <t>ΚΥΡΙΑΖΗ ΚΑΛΛΙΟΠΗ</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>20726.04</v>
+        <v>13210.46</v>
       </c>
       <c r="D34" t="n">
-        <v>688.84</v>
+        <v>218.56</v>
       </c>
       <c r="E34" t="n">
-        <v>970.5700000000001</v>
+        <v>231.78</v>
       </c>
       <c r="F34" t="n">
-        <v>22385.45</v>
+        <v>13660.8</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>0195</t>
+          <t>0044</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>ΚΡΟΝΤΗΡΗΣ ΔΗΜΗΤΡΙΟΣ</t>
+          <t>ΚΥΡΙΑΚΑΚΗΣ ΚΥΡΙΑΚΟΣ</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>7461</v>
+        <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>157.64</v>
+        <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="F35" t="n">
-        <v>7678.64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>1173</t>
+          <t>0227</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>ΚΥΡΙΑΖΗ ΚΑΛΛΙΟΠΗ</t>
+          <t>ΛΕΒΕΝΤΑΚΗ ΜΑΡΙΑ</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>15069.66</v>
+        <v>9837.280000000001</v>
       </c>
       <c r="D36" t="n">
-        <v>376.72</v>
+        <v>184.58</v>
       </c>
       <c r="E36" t="n">
-        <v>580.72</v>
+        <v>0</v>
       </c>
       <c r="F36" t="n">
-        <v>16027.1</v>
+        <v>10021.86</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1153</t>
+          <t>0659</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>ΛΑΓΟΥΔΗ Κ - ΚΑΡΑΓΙΑΝΝΗ Ν. ΣΦ ΟΕ</t>
+          <t>ΛΙΟΔΑΚΗ ΣΤΑΥΡΩΤΗ &amp; ΣΙΑ ΟΕ</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>12243.99</v>
       </c>
       <c r="D37" t="n">
-        <v>-2.98</v>
+        <v>536.3099999999999</v>
       </c>
       <c r="E37" t="n">
-        <v>0</v>
+        <v>20.8</v>
       </c>
       <c r="F37" t="n">
-        <v>-2.98</v>
+        <v>12801.1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>0227</t>
+          <t>1091</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>ΛΕΒΕΝΤΑΚΗ ΜΑΡΙΑ</t>
+          <t>ΜΑΚΡΥΓΙΑΝΝΑΚΗΣ Ζ. ΚΩΝΣΤΑΝΤΙΝΟΣ &amp; ΣΙΑ ΟΕ</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>17916.17</v>
+        <v>6434.67</v>
       </c>
       <c r="D38" t="n">
-        <v>148.25</v>
+        <v>326.65</v>
       </c>
       <c r="E38" t="n">
-        <v>0</v>
+        <v>99.42</v>
       </c>
       <c r="F38" t="n">
-        <v>18064.42</v>
+        <v>6860.74</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>0659</t>
+          <t>0821</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>ΛΙΟΔΑΚΗ ΣΤΑΥΡΩΤΗ &amp; ΣΙΑ ΟΕ</t>
+          <t>ΜΑΛΕΦΙΤΣΑΚΗΣ ΕΜΜΑΝ.ΓΡ.</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>15088.62</v>
+        <v>10903.59</v>
       </c>
       <c r="D39" t="n">
-        <v>333.82</v>
+        <v>433.97</v>
       </c>
       <c r="E39" t="n">
-        <v>17.65</v>
+        <v>112.58</v>
       </c>
       <c r="F39" t="n">
-        <v>15440.09</v>
+        <v>11450.14</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1091</t>
+          <t>1089</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>ΜΑΚΡΥΓΙΑΝΝΑΚΗΣ Ζ. ΚΩΝΣΤΑΝΤΙΝΟΣ &amp; ΣΙΑ ΟΕ</t>
+          <t>ΜΑΛΟΥΠΟΣ Γ. ΝΙΚΟΛΑΟΣ</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>6631.56</v>
+        <v>6651.63</v>
       </c>
       <c r="D40" t="n">
-        <v>407.19</v>
+        <v>13.01</v>
       </c>
       <c r="E40" t="n">
-        <v>176.49</v>
+        <v>0</v>
       </c>
       <c r="F40" t="n">
-        <v>7215.24</v>
+        <v>6664.64</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>0821</t>
+          <t>0673</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>ΜΑΛΕΦΙΤΣΑΚΗΣ ΕΜΜΑΝ.ΓΡ.</t>
+          <t>ΜΑΡΟΥΛΑΚΗ ΑΛΙΚΗ</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>12926.8</v>
+        <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>348.69</v>
+        <v>26.8</v>
       </c>
       <c r="E41" t="n">
-        <v>188.16</v>
+        <v>0</v>
       </c>
       <c r="F41" t="n">
-        <v>13463.65</v>
+        <v>26.8</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>1089</t>
+          <t>0267</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>ΜΑΛΟΥΠΟΣ Γ. ΝΙΚΟΛΑΟΣ</t>
+          <t>ΜΕΛΙΣΟΥΡΓΑΚΗ ΚΥΡΙΑΚΗ</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1289.62</v>
+        <v>3409.68</v>
       </c>
       <c r="D42" t="n">
-        <v>-159.94</v>
+        <v>160.65</v>
       </c>
       <c r="E42" t="n">
         <v>0</v>
       </c>
       <c r="F42" t="n">
-        <v>1129.68</v>
+        <v>3570.33</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>0673</t>
+          <t>0251</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>ΜΑΡΟΥΛΑΚΗ ΑΛΙΚΗ</t>
+          <t>ΜΕΝΕΓΑΚΗ Ε.-ΜΩΥΣΑΚΗ Λ. ΟΕ</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>19666.2</v>
       </c>
       <c r="D43" t="n">
-        <v>42</v>
+        <v>130.34</v>
       </c>
       <c r="E43" t="n">
-        <v>0</v>
+        <v>257.56</v>
       </c>
       <c r="F43" t="n">
-        <v>42</v>
+        <v>20054.1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>0267</t>
+          <t>0079</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>ΜΕΛΙΣΟΥΡΓΑΚΗ ΚΥΡΙΑΚΗ</t>
+          <t>ΜΕΡΩΝΙΑΝΑΚΗ Ζ. ΣΤΥΛΙΑΝΗ</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>4390.61</v>
+        <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>136.57</v>
+        <v>53</v>
       </c>
       <c r="E44" t="n">
         <v>0</v>
       </c>
       <c r="F44" t="n">
-        <v>4527.179999999999</v>
+        <v>53</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>0251</t>
+          <t>1170</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>ΜΕΝΕΓΑΚΗ Ε.-ΜΩΥΣΑΚΗ Λ. ΟΕ</t>
+          <t>ΜΕΤΑΞΑΚΗΣ ΓΕΩΡΓΙΟΣ</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>25402.68</v>
+        <v>23913.2</v>
       </c>
       <c r="D45" t="n">
-        <v>-48.45</v>
+        <v>359.38</v>
       </c>
       <c r="E45" t="n">
-        <v>285.93</v>
+        <v>382.93</v>
       </c>
       <c r="F45" t="n">
-        <v>25640.16</v>
+        <v>24655.51</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>0079</t>
+          <t>0276</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>ΜΕΡΩΝΙΑΝΑΚΗ Ζ. ΣΤΥΛΙΑΝΗ</t>
+          <t>ΜΙΧΕΛΑΚΗΣ ΕΜΜΑΝΟΥΗΛ ΚΑΙ ΣΙΑ ΟΕ</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>12432.54</v>
       </c>
       <c r="D46" t="n">
-        <v>-69.17</v>
+        <v>304.33</v>
       </c>
       <c r="E46" t="n">
-        <v>0</v>
+        <v>148.18</v>
       </c>
       <c r="F46" t="n">
-        <v>-69.17</v>
+        <v>12885.05</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>1170</t>
+          <t>0969</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>ΜΕΤΑΞΑΚΗΣ ΓΕΩΡΓΙΟΣ</t>
+          <t>ΜΠΙΝΙΧΑΚΗΣ ΣΤΑΥΡΟΣ</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>21056.4</v>
+        <v>14364.45</v>
       </c>
       <c r="D47" t="n">
-        <v>416.35</v>
+        <v>239.93</v>
       </c>
       <c r="E47" t="n">
-        <v>493.94</v>
+        <v>174.96</v>
       </c>
       <c r="F47" t="n">
-        <v>21966.69</v>
+        <v>14779.34</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>0276</t>
+          <t>0305</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>ΜΙΧΕΛΑΚΗΣ ΕΜΜΑΝΟΥΗΛ ΚΑΙ ΣΙΑ ΟΕ</t>
+          <t>ΜΠΙΤΖΑΡΑΚΗ ΚΑΛΛΙΟΠΗ</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>13515.84</v>
+        <v>772.17</v>
       </c>
       <c r="D48" t="n">
-        <v>207.22</v>
+        <v>131.03</v>
       </c>
       <c r="E48" t="n">
-        <v>117.2</v>
+        <v>0</v>
       </c>
       <c r="F48" t="n">
-        <v>13840.26</v>
+        <v>903.1999999999999</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>0969</t>
+          <t>0264</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>ΜΠΙΝΙΧΑΚΗΣ ΣΤΑΥΡΟΣ</t>
+          <t>ΝΙΚΟΛΑΙΔΗΣ Γ. ΕΜΜΑΝΟΥΗΛ</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>17579.21</v>
+        <v>15551.72</v>
       </c>
       <c r="D49" t="n">
-        <v>-33.53</v>
+        <v>895.58</v>
       </c>
       <c r="E49" t="n">
-        <v>159.55</v>
+        <v>174.79</v>
       </c>
       <c r="F49" t="n">
-        <v>17705.23</v>
+        <v>16622.09</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>0305</t>
+          <t>0061</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>ΜΠΙΤΖΑΡΑΚΗ ΚΑΛΛΙΟΠΗ</t>
+          <t>ΝΙΚΟΛΑΙΔΗΣ ΓΕΩΡΓ.ΝΙΚΟΛΑΟΣ</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>1193.61</v>
+        <v>12509.22</v>
       </c>
       <c r="D50" t="n">
-        <v>222.16</v>
+        <v>711.29</v>
       </c>
       <c r="E50" t="n">
-        <v>0</v>
+        <v>251</v>
       </c>
       <c r="F50" t="n">
-        <v>1415.77</v>
+        <v>13471.51</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>0264</t>
+          <t>0443</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>ΝΙΚΟΛΑΙΔΗΣ Γ. ΕΜΜΑΝΟΥΗΛ</t>
+          <t>ΞΥΛΟΥΡΗ ΕΙΡΗΝΗ</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>18635.67</v>
+        <v>8891.08</v>
       </c>
       <c r="D51" t="n">
-        <v>1065.68</v>
+        <v>216.15</v>
       </c>
       <c r="E51" t="n">
-        <v>187.44</v>
+        <v>24.7</v>
       </c>
       <c r="F51" t="n">
-        <v>19888.79</v>
+        <v>9131.93</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>0061</t>
+          <t>0727</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>ΝΙΚΟΛΑΙΔΗΣ ΓΕΩΡΓ.ΝΙΚΟΛΑΟΣ</t>
+          <t>ΠΑΝΑΓΙΩΤΑΚΗ ΠΕΛΑΓΙΑ</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>14682.84</v>
+        <v>8253.360000000001</v>
       </c>
       <c r="D52" t="n">
-        <v>768.35</v>
+        <v>107.88</v>
       </c>
       <c r="E52" t="n">
-        <v>1168.32</v>
+        <v>0</v>
       </c>
       <c r="F52" t="n">
-        <v>16619.51</v>
+        <v>8361.24</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>0443</t>
+          <t>0321</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>ΞΥΛΟΥΡΗ ΕΙΡΗΝΗ</t>
+          <t>ΠΑΠΑΔΑΚΗΣ ΑΝΤΩΝΙΟΣ &amp; ΣΙΑ ΕΕ</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>14852.47</v>
+        <v>1733.26</v>
       </c>
       <c r="D53" t="n">
-        <v>283.9</v>
+        <v>329.46</v>
       </c>
       <c r="E53" t="n">
-        <v>37.46</v>
+        <v>397.44</v>
       </c>
       <c r="F53" t="n">
-        <v>15173.83</v>
+        <v>2460.16</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>0727</t>
+          <t>0462</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>ΠΑΝΑΓΙΩΤΑΚΗ ΠΕΛΑΓΙΑ</t>
+          <t>ΠΑΠΑΔΑΚΗΣ ΝΙΚΟΛΑΟΣ</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>7722.59</v>
+        <v>7481.61</v>
       </c>
       <c r="D54" t="n">
-        <v>156.75</v>
+        <v>183.14</v>
       </c>
       <c r="E54" t="n">
-        <v>55.2</v>
+        <v>23.59</v>
       </c>
       <c r="F54" t="n">
-        <v>7934.54</v>
+        <v>7688.34</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>0321</t>
+          <t>0322</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>ΠΑΠΑΔΑΚΗΣ ΑΝΤΩΝΙΟΣ &amp; ΣΙΑ ΕΕ</t>
+          <t>ΠΑΠΑΔΟΓΙΩΡΓΑΚΗ ΜΑΡΙΑ</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>24664.01</v>
+        <v>11849.44</v>
       </c>
       <c r="D55" t="n">
-        <v>-117</v>
+        <v>288.11</v>
       </c>
       <c r="E55" t="n">
-        <v>131</v>
+        <v>113.07</v>
       </c>
       <c r="F55" t="n">
-        <v>24678.01</v>
+        <v>12250.62</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>0462</t>
+          <t>0103</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>ΠΑΠΑΔΑΚΗΣ ΝΙΚΟΛΑΟΣ</t>
+          <t>ΠΑΠΑΔΟΚΩΣΤΑΚΗΣ ΕΜΜΑΝΟΥΗΛ</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>10114.77</v>
+        <v>5713.47</v>
       </c>
       <c r="D56" t="n">
-        <v>201.96</v>
+        <v>33.07</v>
       </c>
       <c r="E56" t="n">
-        <v>124.64</v>
+        <v>68.09999999999999</v>
       </c>
       <c r="F56" t="n">
-        <v>10441.37</v>
+        <v>5814.64</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>0322</t>
+          <t>0464</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>ΠΑΠΑΔΟΓΙΩΡΓΑΚΗ ΜΑΡΙΑ</t>
+          <t>ΠΑΠΑΘΕΟΔΩΡΟΥ ΕΙΡΗΝΗ</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>11397.49</v>
+        <v>29.5</v>
       </c>
       <c r="D57" t="n">
-        <v>372.39</v>
+        <v>15.15</v>
       </c>
       <c r="E57" t="n">
-        <v>175.89</v>
+        <v>0</v>
       </c>
       <c r="F57" t="n">
-        <v>11945.77</v>
+        <v>44.65</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>0103</t>
+          <t>0108</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>ΠΑΠΑΔΟΚΩΣΤΑΚΗΣ ΕΜΜΑΝΟΥΗΛ</t>
+          <t>ΠΕΤΡΟΠΟΥΛΟΥ ΑΝΤΩΝΙΑ</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>5872.34</v>
+        <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>110.87</v>
+        <v>12</v>
       </c>
       <c r="E58" t="n">
-        <v>164.49</v>
+        <v>0</v>
       </c>
       <c r="F58" t="n">
-        <v>6147.7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>0464</t>
+          <t>0144</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>ΠΑΠΑΘΕΟΔΩΡΟΥ ΕΙΡΗΝΗ</t>
+          <t>ΠΟΛΙΤΑΚΗΣ ΕΜΜΑΝΟΥΗΛ</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>57.44</v>
+        <v>5829.45</v>
       </c>
       <c r="D59" t="n">
-        <v>27.09</v>
+        <v>204.53</v>
       </c>
       <c r="E59" t="n">
-        <v>0</v>
+        <v>143.98</v>
       </c>
       <c r="F59" t="n">
-        <v>84.53</v>
+        <v>6177.959999999999</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>0144</t>
+          <t>1147</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>ΠΟΛΙΤΑΚΗΣ ΕΜΜΑΝΟΥΗΛ</t>
+          <t>ΠΡΑΤΙΚΑΚΗ ΕΥΑΓ &amp; ΧΑΛΚΙΑΔΑΚΗΣ Γ.-ΚΩΝ.ΝΟΣ ΣΦ ΟΕ</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>6526.33</v>
+        <v>13560.33</v>
       </c>
       <c r="D60" t="n">
-        <v>241.2</v>
+        <v>680.61</v>
       </c>
       <c r="E60" t="n">
-        <v>226.84</v>
+        <v>158.9</v>
       </c>
       <c r="F60" t="n">
-        <v>6994.37</v>
+        <v>14399.84</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>0365</t>
+          <t>0099</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>ΠΟΛΙΤΑΚΗΣ ΣΤΥΛΙΑΝΟΣ</t>
+          <t>ΠΡΙΝΑΡΗΣ ΓΕΩΡΓΙΟΣ</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>1648.2</v>
+        <v>9832.940000000001</v>
       </c>
       <c r="D61" t="n">
-        <v>88.51000000000001</v>
+        <v>235.18</v>
       </c>
       <c r="E61" t="n">
-        <v>0</v>
+        <v>77.52</v>
       </c>
       <c r="F61" t="n">
-        <v>1736.71</v>
+        <v>10145.64</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>1147</t>
+          <t>1143</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>ΠΡΑΤΙΚΑΚΗ ΕΥΑΓ &amp; ΧΑΛΚΙΑΔΑΚΗΣ Γ.-ΚΩΝ.ΝΟΣ ΣΦ ΟΕ</t>
+          <t>ΡΙΖΙΚΙΑΝΟΣ ΣΤΥΛΙΑΝΟΣ</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>14272.06</v>
+        <v>16166.87</v>
       </c>
       <c r="D62" t="n">
-        <v>760.4299999999999</v>
+        <v>327.42</v>
       </c>
       <c r="E62" t="n">
-        <v>229.2</v>
+        <v>432.86</v>
       </c>
       <c r="F62" t="n">
-        <v>15261.69</v>
+        <v>16927.15</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>0099</t>
+          <t>0376</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>ΠΡΙΝΑΡΗΣ ΓΕΩΡΓΙΟΣ</t>
+          <t>ΡΟΥΣΑΚΗ ΜΑΡΙΝΑ-ΚΑΛΛΙΤΣΑΚΗ</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>7852.12</v>
+        <v>10167.43</v>
       </c>
       <c r="D63" t="n">
-        <v>233.13</v>
+        <v>340.36</v>
       </c>
       <c r="E63" t="n">
-        <v>202.07</v>
+        <v>129.32</v>
       </c>
       <c r="F63" t="n">
-        <v>8287.32</v>
+        <v>10637.11</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>1143</t>
+          <t>0380</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>ΡΙΖΙΚΙΑΝΟΣ ΣΤΥΛΙΑΝΟΣ</t>
+          <t>ΣΑΛΟΥΣΤΡΟΥ ΕΛΕΝΗ</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>12103.13</v>
+        <v>5095.53</v>
       </c>
       <c r="D64" t="n">
-        <v>53.23</v>
+        <v>171.73</v>
       </c>
       <c r="E64" t="n">
-        <v>296.6</v>
+        <v>18.6</v>
       </c>
       <c r="F64" t="n">
-        <v>12452.96</v>
+        <v>5285.86</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>0377</t>
+          <t>0092</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>ΡΟΥΜΠΕΛΑΚΗΣ ΝΙΚΟΛΑΟΣ</t>
+          <t>ΣΑΡΡΗΣ Κ. ΝΙΚΟΛΑΟΣ</t>
         </is>
       </c>
       <c r="C65" t="n">
         <v>0</v>
       </c>
       <c r="D65" t="n">
-        <v>-8</v>
+        <v>34.2</v>
       </c>
       <c r="E65" t="n">
         <v>0</v>
       </c>
       <c r="F65" t="n">
-        <v>-8</v>
+        <v>34.2</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>0376</t>
+          <t>0386</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>ΡΟΥΣΑΚΗ ΜΑΡΙΝΑ-ΚΑΛΛΙΤΣΑΚΗ</t>
+          <t>ΣΜΑΡΓΙΑΝΝΑΚΗΣ ΣΤΑΥΡΟΣ &amp; ΣΙΑ ΕΕ</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>10313.16</v>
+        <v>9576.290000000001</v>
       </c>
       <c r="D66" t="n">
-        <v>462.45</v>
+        <v>212.99</v>
       </c>
       <c r="E66" t="n">
-        <v>71.98</v>
+        <v>30</v>
       </c>
       <c r="F66" t="n">
-        <v>10847.59</v>
+        <v>9819.280000000001</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>0380</t>
+          <t>1118</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>ΣΑΛΟΥΣΤΡΟΥ ΕΛΕΝΗ</t>
+          <t>ΣΤΑΜΑΤΑΚΗ ΑΘΗΝΑ-ΜΑΡΙΑ</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>5867.01</v>
+        <v>11747.55</v>
       </c>
       <c r="D67" t="n">
-        <v>-6.76</v>
+        <v>87.8</v>
       </c>
       <c r="E67" t="n">
-        <v>28.17</v>
+        <v>92.29000000000001</v>
       </c>
       <c r="F67" t="n">
-        <v>5888.42</v>
+        <v>11927.64</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>0092</t>
+          <t>0842</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>ΣΑΡΡΗΣ Κ. ΝΙΚΟΛΑΟΣ</t>
+          <t>ΣΤΕΦΑΝΑΚΗ ΕΛΕΝΗ</t>
         </is>
       </c>
       <c r="C68" t="n">
         <v>0</v>
       </c>
       <c r="D68" t="n">
-        <v>-109.01</v>
+        <v>11.36</v>
       </c>
       <c r="E68" t="n">
         <v>0</v>
       </c>
       <c r="F68" t="n">
-        <v>-109.01</v>
+        <v>11.36</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>0388</t>
+          <t>0069</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>ΣΙΓΑΝΟΣ ΕΜΜΑΝΟΥΗΛ &amp; ΣΙΑ ΟΕ</t>
+          <t>ΣΤΕΦΑΝΑΚΗ ΜΑΡΙΑ &amp; ΣΙΑ ΟΕ</t>
         </is>
       </c>
       <c r="C69" t="n">
         <v>0</v>
       </c>
       <c r="D69" t="n">
-        <v>11.29</v>
+        <v>0</v>
       </c>
       <c r="E69" t="n">
         <v>0</v>
       </c>
       <c r="F69" t="n">
-        <v>11.29</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>0386</t>
+          <t>0122</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>ΣΜΑΡΓΙΑΝΝΑΚΗΣ ΣΤΑΥΡΟΣ &amp; ΣΙΑ ΕΕ</t>
+          <t>ΣΤΕΦΑΝΑΚΗ ΟΛΓΑ &amp; ΣΙΑ ΟΕ</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>11288.62</v>
+        <v>0</v>
       </c>
       <c r="D70" t="n">
-        <v>-27.26</v>
+        <v>49.94</v>
       </c>
       <c r="E70" t="n">
-        <v>148.21</v>
+        <v>0</v>
       </c>
       <c r="F70" t="n">
-        <v>11409.57</v>
+        <v>49.94</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>1118</t>
+          <t>0078</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>ΣΤΑΜΑΤΑΚΗ ΑΘΗΝΑ-ΜΑΡΙΑ</t>
+          <t>ΣΤΕΦΑΝΑΚΗΣ ΣΤ. ΕΜΜΑΝΟΥΗΛ</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>12281.86</v>
+        <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>158.58</v>
+        <v>12</v>
       </c>
       <c r="E71" t="n">
-        <v>206.96</v>
+        <v>0</v>
       </c>
       <c r="F71" t="n">
-        <v>12647.4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>0842</t>
+          <t>1175</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>ΣΤΕΦΑΝΑΚΗ ΕΛΕΝΗ</t>
+          <t>ΣΦ ΔΑΜΗΛΑΚΗ ΑΝΑΣΤΑΣΑΚΗ ΑΙΚΑΤΕΡΙΝΗ &amp; ΑΝΑΣΤΑΣΑΚΗΣ ΚΩΝΣΤΑΝΤΙΝΟΣ ΟΕ</t>
         </is>
       </c>
       <c r="C72" t="n">
         <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>-199.17</v>
+        <v>51.3</v>
       </c>
       <c r="E72" t="n">
         <v>0</v>
       </c>
       <c r="F72" t="n">
-        <v>-199.17</v>
+        <v>51.3</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>0069</t>
+          <t>0151</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>ΣΤΕΦΑΝΑΚΗ ΜΑΡΙΑ &amp; ΣΙΑ ΟΕ</t>
+          <t>ΣΦ ΚΑΝΑΚΑΚΗΣ Λ. - Κ. ΤΕΤΟΚΑ ΚΑΙ ΣΙΑ ΟΕ</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>2158.1</v>
       </c>
       <c r="D73" t="n">
-        <v>-120.04</v>
+        <v>96.2</v>
       </c>
       <c r="E73" t="n">
-        <v>0</v>
+        <v>9.93</v>
       </c>
       <c r="F73" t="n">
-        <v>-120.04</v>
+        <v>2264.23</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>0122</t>
+          <t>1176</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>ΣΤΕΦΑΝΑΚΗ ΟΛΓΑ &amp; ΣΙΑ ΟΕ</t>
+          <t>ΣΦ ΚΤΙΣΤΑΚΗ ΑΓΓΕΛΙΚΗ ΜΑΚΡΥΓΙΑΝΝΑΚΗΣ ΠΟΛΥΧΡΟΝΗΣ ΟΕ</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>10593.4</v>
       </c>
       <c r="D74" t="n">
-        <v>-208.23</v>
+        <v>122.71</v>
       </c>
       <c r="E74" t="n">
-        <v>0</v>
+        <v>124.09</v>
       </c>
       <c r="F74" t="n">
-        <v>-208.23</v>
+        <v>10840.2</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>0483</t>
+          <t>0094</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>ΣΦ ΒΟΓΙΑΤΖΗΣ ΙΩΑΝΝΗΣ &amp; ΒΟΓΙΑΤΖΗ ΑΓΓΕΛΙΚΗ ΟΕ</t>
+          <t>ΣΦ ΠΑΠΑΔΟΚΩΣΤΑΚΗΣ Φ.-ΠΑΠΑΔΟΚΩΣΤΑΚΗΣ Γ. ΟΕ</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>0</v>
+        <v>10593.87</v>
       </c>
       <c r="D75" t="n">
-        <v>29.43</v>
+        <v>39.61</v>
       </c>
       <c r="E75" t="n">
-        <v>0</v>
+        <v>223.69</v>
       </c>
       <c r="F75" t="n">
-        <v>29.43</v>
+        <v>10857.17</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>1175</t>
+          <t>0361</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>ΣΦ ΔΑΜΗΛΑΚΗ ΑΝΑΣΤΑΣΑΚΗ ΑΙΚΑΤΕΡΙΝΗ &amp; ΑΝΑΣΤΑΣΑΚΗΣ ΚΩΝΣΤΑΝΤΙΝΟΣ ΟΕ</t>
+          <t>ΣΦ ΠΛΑΚΟΓΙΑΝΝΑΚΗΣ ΜΙΧΑΗΛ &amp; ΠΛΑΚΟΓΙΑΝΝΑΚΗΣ ΓΕΩΡΓΙΟΣ Ο.Ε.</t>
         </is>
       </c>
       <c r="C76" t="n">
         <v>0</v>
       </c>
       <c r="D76" t="n">
-        <v>0</v>
+        <v>625.04</v>
       </c>
       <c r="E76" t="n">
-        <v>0</v>
+        <v>42.09</v>
       </c>
       <c r="F76" t="n">
-        <v>0</v>
+        <v>667.13</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>0151</t>
+          <t>1477</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>ΣΦ ΚΑΝΑΚΑΚΗΣ Λ. - Κ. ΤΕΤΟΚΑ ΚΑΙ ΣΙΑ ΟΕ</t>
+          <t>ΣΦ ΠΟΛΙΤΑΚΗΣ ΣΤΥΛΙΑΝΟΣ-ΠΟΛΙΤΑΚΗ ΠΑΡΑΣΚΕΥΗ ΟΕ</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>2167.64</v>
+        <v>1440.28</v>
       </c>
       <c r="D77" t="n">
-        <v>111.33</v>
+        <v>130.66</v>
       </c>
       <c r="E77" t="n">
-        <v>9.66</v>
+        <v>2.5</v>
       </c>
       <c r="F77" t="n">
-        <v>2288.63</v>
+        <v>1573.44</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>1176</t>
+          <t>1187</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>ΣΦ ΚΤΙΣΤΑΚΗ ΑΓΓΕΛΙΚΗ ΜΑΚΡΥΓΙΑΝΝΑΚΗΣ ΠΟΛΥΧΡΟΝΗΣ ΟΕ</t>
+          <t>ΣΦ ΣΚΟΝΤΙΝΗ ΞΕΝΗ &amp; ΧΟΥΡΣΑΝΙΔΗΣ ΠΑΡΑΣΧΟΣ ΟΕ</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>12559.27</v>
+        <v>0</v>
       </c>
       <c r="D78" t="n">
-        <v>50.03</v>
+        <v>48.73</v>
       </c>
       <c r="E78" t="n">
-        <v>109.45</v>
+        <v>0</v>
       </c>
       <c r="F78" t="n">
-        <v>12718.75</v>
+        <v>48.73</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>0277</t>
+          <t>0074</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>ΣΦ ΝΙΚΟΛΑΚΟΠΟΥΛΟΥ ΜΑΡΙΑ&amp;ΜΑΥΡΟΚΟΥΚΟΥΛΑΚΗ ΕΙΡΗΑΝΝΑ ΟΕ</t>
+          <t>ΤΣΑΟΥΛΗΣ ΓΕΩΡΓΙΟΣ &amp; ΣΙΑ ΟΕ</t>
         </is>
       </c>
       <c r="C79" t="n">
         <v>0</v>
       </c>
       <c r="D79" t="n">
-        <v>-95.04000000000001</v>
+        <v>33.32</v>
       </c>
       <c r="E79" t="n">
         <v>0</v>
       </c>
       <c r="F79" t="n">
-        <v>-95.04000000000001</v>
+        <v>33.32</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>0094</t>
+          <t>0833</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>ΣΦ ΠΑΠΑΔΟΚΩΣΤΑΚΗΣ Φ.-ΠΑΠΑΔΟΚΩΣΤΑΚΗΣ Γ. ΟΕ</t>
+          <t>ΦΟΥΚΑΚΗ ΜΑΡΙΑ ΕΛΕΥΘΕΡΙΟΥ</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>11450.32</v>
+        <v>13762.36</v>
       </c>
       <c r="D80" t="n">
-        <v>29.39</v>
+        <v>220.25</v>
       </c>
       <c r="E80" t="n">
-        <v>351.82</v>
+        <v>0</v>
       </c>
       <c r="F80" t="n">
-        <v>11831.53</v>
+        <v>13982.61</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>0361</t>
+          <t>1200</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>ΣΦ ΠΛΑΚΟΓΙΑΝΝΑΚΗΣ ΜΙΧΑΗΛ &amp; ΠΛΑΚΟΓΙΑΝΝΑΚΗΣ ΓΕΩΡΓΙΟΣ Ο.Ε.</t>
+          <t>ΦΟΥΛΕΔΑΚΗΣ Μ ΔΗΜΗΤΡΙΟΣ</t>
         </is>
       </c>
       <c r="C81" t="n">
         <v>0</v>
       </c>
       <c r="D81" t="n">
-        <v>691.49</v>
+        <v>159.33</v>
       </c>
       <c r="E81" t="n">
-        <v>429.68</v>
+        <v>0</v>
       </c>
       <c r="F81" t="n">
-        <v>1121.17</v>
+        <v>159.33</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>1477</t>
+          <t>1103</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>ΣΦ ΠΟΛΙΤΑΚΗΣ ΣΤΥΛΙΑΝΟΣ-ΠΟΛΙΤΑΚΗ ΠΑΡΑΣΚΕΥΗ ΟΕ</t>
+          <t>ΧΑΜΑΛΑΚΗ ΧΡΥΣΟΥΛΑ</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>1139.05</v>
+        <v>2422.32</v>
       </c>
       <c r="D82" t="n">
-        <v>9.42</v>
+        <v>5.91</v>
       </c>
       <c r="E82" t="n">
-        <v>26.24</v>
+        <v>0</v>
       </c>
       <c r="F82" t="n">
-        <v>1174.71</v>
+        <v>2428.23</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>1187</t>
+          <t>1111</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>ΣΦ ΣΚΟΝΤΙΝΗ ΞΕΝΗ &amp; ΧΟΥΡΣΑΝΙΔΗΣ ΠΑΡΑΣΧΟΣ ΟΕ</t>
+          <t>ΧΑΝΙΩΤΑΚΗ Ε. ΕΥΑΓΓΕΛΙΑ</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>8895.48</v>
       </c>
       <c r="D83" t="n">
-        <v>129.84</v>
+        <v>161.54</v>
       </c>
       <c r="E83" t="n">
-        <v>0</v>
+        <v>51.02</v>
       </c>
       <c r="F83" t="n">
-        <v>129.84</v>
+        <v>9108.040000000001</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>0074</t>
+          <t>0440</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>ΤΣΑΟΥΛΗΣ ΓΕΩΡΓΙΟΣ &amp; ΣΙΑ ΟΕ</t>
+          <t>ΧΑΡΑΛΑΜΠΑΚΗ ΝΟΥΛΑ ΓΙΩΤΑ</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
+        <v>8503.07</v>
       </c>
       <c r="D84" t="n">
-        <v>-5.68</v>
+        <v>340.61</v>
       </c>
       <c r="E84" t="n">
-        <v>0</v>
+        <v>112.09</v>
       </c>
       <c r="F84" t="n">
-        <v>-5.68</v>
+        <v>8955.77</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>0833</t>
+          <t>0017</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>ΦΟΥΚΑΚΗ ΜΑΡΙΑ ΕΛΕΥΘΕΡΙΟΥ</t>
+          <t>ΧΑΡΑΛΑΜΠΑΚΗΣ ΧΡΗΣΤΟΣ &amp; ΘΕΟΔΩΡΟΣ ΟΕ</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>14412.58</v>
+        <v>10050.18</v>
       </c>
       <c r="D85" t="n">
-        <v>82.95</v>
+        <v>735.61</v>
       </c>
       <c r="E85" t="n">
-        <v>39.24</v>
+        <v>138.04</v>
       </c>
       <c r="F85" t="n">
-        <v>14534.77</v>
+        <v>10923.83</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>1200</t>
+          <t>0693</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>ΦΟΥΛΕΔΑΚΗΣ Μ ΔΗΜΗΤΡΙΟΣ</t>
+          <t>ΧΑΤΖΑΚΗΣ ΙΩΑΝΝΗΣ</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
+        <v>20151.72</v>
       </c>
       <c r="D86" t="n">
-        <v>283</v>
+        <v>1271.45</v>
       </c>
       <c r="E86" t="n">
-        <v>15</v>
+        <v>302.34</v>
       </c>
       <c r="F86" t="n">
-        <v>298</v>
+        <v>21725.51</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>0792</t>
+          <t>1149</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>ΧΑΛΚΙΑΔΑΚΗΣ ΑΝΤΩΝΗΣ</t>
+          <t>ΧΑΤΖΗΔΑΚΗ ΑΝΑΣΤΑΣΙΑ ΕΕ</t>
         </is>
       </c>
       <c r="C87" t="n">
         <v>0</v>
       </c>
       <c r="D87" t="n">
-        <v>0</v>
+        <v>60.24</v>
       </c>
       <c r="E87" t="n">
-        <v>0</v>
+        <v>25.55</v>
       </c>
       <c r="F87" t="n">
-        <v>0</v>
+        <v>85.79000000000001</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>1103</t>
+          <t>0413</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>ΧΑΜΑΛΑΚΗ ΧΡΥΣΟΥΛΑ</t>
+          <t>ΧΑΤΖΗΔΑΚΗ ΚΑΛΛΙΟΠΗ ΧΑΤΖΑΚΗΣ ΜΙΧΑΗΛ &amp; ΣΙΑ ΟΕ</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>2916.3</v>
+        <v>5272.48</v>
       </c>
       <c r="D88" t="n">
-        <v>82.20999999999999</v>
+        <v>63.74</v>
       </c>
       <c r="E88" t="n">
-        <v>0</v>
+        <v>21.29</v>
       </c>
       <c r="F88" t="n">
-        <v>2998.51</v>
+        <v>5357.509999999999</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>1111</t>
+          <t>0811</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>ΧΑΝΙΩΤΑΚΗ Ε. ΕΥΑΓΓΕΛΙΑ</t>
+          <t>ΧΑΤΖΙΔΑΚΗΣ ΕΠΑΜΕΙΝΩΝΔΑΣ</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>8176.93</v>
+        <v>0</v>
       </c>
       <c r="D89" t="n">
-        <v>3.66</v>
+        <v>0</v>
       </c>
       <c r="E89" t="n">
         <v>0</v>
       </c>
       <c r="F89" t="n">
-        <v>8180.59</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>0440</t>
+          <t>0467</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>ΧΑΡΑΛΑΜΠΑΚΗ ΝΟΥΛΑ ΓΙΩΤΑ</t>
+          <t>ΧΟΥΣΤΟΥΛΑΚΗΣ ΕΜΜΑΝΟΥΗΛ</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>9386.629999999999</v>
+        <v>11054.97</v>
       </c>
       <c r="D90" t="n">
-        <v>360.14</v>
+        <v>196.93</v>
       </c>
       <c r="E90" t="n">
-        <v>54.9</v>
+        <v>283.57</v>
       </c>
       <c r="F90" t="n">
-        <v>9801.669999999998</v>
+        <v>11535.47</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>0017</t>
+          <t>1085</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>ΧΑΡΑΛΑΜΠΑΚΗΣ ΧΡΗΣΤΟΣ &amp; ΘΕΟΔΩΡΟΣ ΟΕ</t>
+          <t>ΧΡΙΣΤΟΔΟΥΛΑΚΗΣ ΑΛΕΞ. &amp; ΧΡΙΣΤΟΔΟΥΛΑΚΗΣ ΓΕΩΡΓ. ΣΦ ΟΕ</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>11133.89</v>
+        <v>19132.42</v>
       </c>
       <c r="D91" t="n">
-        <v>939.2</v>
+        <v>448.31</v>
       </c>
       <c r="E91" t="n">
-        <v>165.57</v>
+        <v>257.97</v>
       </c>
       <c r="F91" t="n">
-        <v>12238.66</v>
+        <v>19838.7</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>0049</t>
+          <t>0470</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>ΧΑΡΚΙΑΝΑΚΗΣ ΝΙΚΟΛΑΟΣ</t>
+          <t>ΨΑΛΤΑΚΗΣ ΣΤΥΛΙΑΝΟΣ</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>0</v>
+        <v>9071.91</v>
       </c>
       <c r="D92" t="n">
-        <v>-81.01000000000001</v>
+        <v>138.44</v>
       </c>
       <c r="E92" t="n">
-        <v>0</v>
+        <v>40.44</v>
       </c>
       <c r="F92" t="n">
-        <v>-81.01000000000001</v>
+        <v>9250.790000000001</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>0693</t>
+          <t>0281</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>ΧΑΤΖΑΚΗΣ ΙΩΑΝΝΗΣ</t>
+          <t>ΨΑΡΟΥΔΑΚΗ ΑΝΑΣΤΑΣΙΑ &amp; ΣΙΑ ΟΕ</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>23469.91</v>
+        <v>6371.23</v>
       </c>
       <c r="D93" t="n">
-        <v>1181.19</v>
+        <v>80.78</v>
       </c>
       <c r="E93" t="n">
-        <v>296.53</v>
+        <v>0</v>
       </c>
       <c r="F93" t="n">
-        <v>24947.63</v>
+        <v>6452.009999999999</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>1149</t>
+          <t>094</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>ΧΑΤΖΗΔΑΚΗ ΑΝΑΣΤΑΣΙΑ ΕΕ</t>
+          <t>10000</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>0.53</v>
       </c>
       <c r="D94" t="n">
-        <v>156.71</v>
+        <v>-3.15</v>
       </c>
       <c r="E94" t="n">
-        <v>0</v>
+        <v>4.83</v>
       </c>
       <c r="F94" t="n">
-        <v>156.71</v>
+        <v>2.21</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>0413</t>
+          <t>0272</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>ΧΑΤΖΗΔΑΚΗ ΚΑΛΛΙΟΠΗ ΧΑΤΖΑΚΗΣ ΜΙΧΑΗΛ &amp; ΣΙΑ ΟΕ</t>
+          <t>ΓΑΛΑΝΗ ΠΑΝ. ΜΑΡΙΑ</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>6357.63</v>
+        <v>543.92</v>
       </c>
       <c r="D95" t="n">
-        <v>-170.23</v>
+        <v>149.7</v>
       </c>
       <c r="E95" t="n">
-        <v>209</v>
+        <v>20.8</v>
       </c>
       <c r="F95" t="n">
-        <v>6396.400000000001</v>
+        <v>714.4199999999998</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>0467</t>
+          <t>1169</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>ΧΟΥΣΤΟΥΛΑΚΗΣ ΕΜΜΑΝΟΥΗΛ</t>
+          <t>ΘΕΟΔΩΡΑΚΗΣ Γ. ΑΝΤΩΝΙΟΣ</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>14520.72</v>
+        <v>0</v>
       </c>
       <c r="D96" t="n">
-        <v>317.23</v>
+        <v>18.43</v>
       </c>
       <c r="E96" t="n">
-        <v>402.79</v>
+        <v>0</v>
       </c>
       <c r="F96" t="n">
-        <v>15240.74</v>
+        <v>18.43</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>1085</t>
+          <t>1161</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>ΧΡΙΣΤΟΔΟΥΛΑΚΗΣ ΑΛΕΞ. &amp; ΧΡΙΣΤΟΔΟΥΛΑΚΗΣ ΓΕΩΡΓ. ΣΦ ΟΕ</t>
+          <t>ΘΕΟΔΩΡΙΔΗΣ ΙΟΡΔΑΝΗΣ-ΘΕΟΔΩΡΙΔΗ ΒΑΣΙΛΙΚΗ ΣΦ ΟΕ</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>18892.56</v>
+        <v>4422.45</v>
       </c>
       <c r="D97" t="n">
-        <v>272.17</v>
+        <v>221.44</v>
       </c>
       <c r="E97" t="n">
-        <v>229.71</v>
+        <v>13</v>
       </c>
       <c r="F97" t="n">
-        <v>19394.44</v>
+        <v>4656.889999999999</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>0470</t>
+          <t>1177</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>ΨΑΛΤΑΚΗΣ ΣΤΥΛΙΑΝΟΣ</t>
+          <t>ΛΥΡΑΤΖΑΚΗ ΜΑΡΙΑΝΝΑ</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>9591.610000000001</v>
+        <v>0</v>
       </c>
       <c r="D98" t="n">
-        <v>95.03</v>
+        <v>83.76000000000001</v>
       </c>
       <c r="E98" t="n">
         <v>0</v>
       </c>
       <c r="F98" t="n">
-        <v>9686.640000000001</v>
+        <v>83.76000000000001</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>0281</t>
+          <t>0198</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>ΨΑΡΟΥΔΑΚΗ ΑΝΑΣΤΑΣΙΑ &amp; ΣΙΑ ΟΕ</t>
+          <t>ΜΑΡΚΑΝΤΩΝΑΚΗ ΜΑΡΙΝΑ</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>16021.74</v>
+        <v>255.64</v>
       </c>
       <c r="D99" t="n">
-        <v>42.76</v>
+        <v>14.5</v>
       </c>
       <c r="E99" t="n">
         <v>0</v>
       </c>
       <c r="F99" t="n">
-        <v>16064.5</v>
+        <v>270.14</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>0740</t>
+          <t>1444</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>ΨΥΧΑΡΑΚΗ ΕΥΡΙΔΙΚΗ</t>
+          <t>ΠΑΠΑΔΑΚΗ ΕΥΑΓΓΕΛΙΑ &amp; ΣΙΑ ΕΕ</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>0</v>
+        <v>244.75</v>
       </c>
       <c r="D100" t="n">
-        <v>94.90000000000001</v>
+        <v>63.07</v>
       </c>
       <c r="E100" t="n">
         <v>0</v>
       </c>
       <c r="F100" t="n">
-        <v>94.90000000000001</v>
+        <v>307.82</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>111</t>
+          <t>0173</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>9996</t>
+          <t>ΠΑΠΑΔΑΚΗ ΕΥΑΓΓΕΛΙΑ</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>1.42</v>
+        <v>406.21</v>
       </c>
       <c r="D101" t="n">
-        <v>2.12</v>
+        <v>61.9</v>
       </c>
       <c r="E101" t="n">
-        <v>8.140000000000001</v>
+        <v>0</v>
       </c>
       <c r="F101" t="n">
-        <v>11.68</v>
+        <v>468.11</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>0272</t>
+          <t>1083</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>ΓΑΛΑΝΗ ΠΑΝ. ΜΑΡΙΑ</t>
+          <t>ΤΟΛΟΥΔΗΣ Π. ΜΑΡΚΟΣ</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>484.01</v>
+        <v>0</v>
       </c>
       <c r="D102" t="n">
-        <v>40.06</v>
+        <v>30.63</v>
       </c>
       <c r="E102" t="n">
-        <v>33.32</v>
+        <v>0</v>
       </c>
       <c r="F102" t="n">
-        <v>557.39</v>
+        <v>30.63</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>1169</t>
+          <t>0212</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>ΘΕΟΔΩΡΑΚΗΣ Γ. ΑΝΤΩΝΙΟΣ</t>
+          <t>ΧΑΤΖΙΔΑΚΙ ΕΠΑΜ. ΑΡΓΥΡΗ</t>
         </is>
       </c>
       <c r="C103" t="n">
         <v>0</v>
       </c>
       <c r="D103" t="n">
-        <v>5.27</v>
+        <v>0</v>
       </c>
       <c r="E103" t="n">
         <v>0</v>
       </c>
       <c r="F103" t="n">
-        <v>5.27</v>
-      </c>
-    </row>
-    <row r="104">
-      <c r="A104" t="inlineStr">
-        <is>
-          <t>1161</t>
-        </is>
-      </c>
-      <c r="B104" t="inlineStr">
-        <is>
-          <t>ΘΕΟΔΩΡΙΔΗΣ ΙΟΡΔΑΝΗΣ-ΘΕΟΔΩΡΙΔΗ ΒΑΣΙΛΙΚΗ ΣΦ ΟΕ</t>
-        </is>
-      </c>
-      <c r="C104" t="n">
-        <v>7425.52</v>
-      </c>
-      <c r="D104" t="n">
-        <v>282.02</v>
-      </c>
-      <c r="E104" t="n">
-        <v>74.28</v>
-      </c>
-      <c r="F104" t="n">
-        <v>7781.820000000001</v>
-      </c>
-    </row>
-    <row r="105">
-      <c r="A105" t="inlineStr">
-        <is>
-          <t>2179</t>
-        </is>
-      </c>
-      <c r="B105" t="inlineStr">
-        <is>
-          <t>ΚΩΝΣΤΑ ΜΙΚΕ ΙΩΑΝΝΑ</t>
-        </is>
-      </c>
-      <c r="C105" t="n">
-        <v>0</v>
-      </c>
-      <c r="D105" t="n">
-        <v>0</v>
-      </c>
-      <c r="E105" t="n">
-        <v>0</v>
-      </c>
-      <c r="F105" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106">
-      <c r="A106" t="inlineStr">
-        <is>
-          <t>1177</t>
-        </is>
-      </c>
-      <c r="B106" t="inlineStr">
-        <is>
-          <t>ΛΥΡΑΤΖΑΚΗ ΜΑΡΙΑΝΝΑ</t>
-        </is>
-      </c>
-      <c r="C106" t="n">
-        <v>0</v>
-      </c>
-      <c r="D106" t="n">
-        <v>46.04</v>
-      </c>
-      <c r="E106" t="n">
-        <v>0</v>
-      </c>
-      <c r="F106" t="n">
-        <v>46.04</v>
-      </c>
-    </row>
-    <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>0198</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr">
-        <is>
-          <t>ΜΑΡΚΑΝΤΩΝΑΚΗ ΜΑΡΙΝΑ</t>
-        </is>
-      </c>
-      <c r="C107" t="n">
-        <v>205.32</v>
-      </c>
-      <c r="D107" t="n">
-        <v>31.44</v>
-      </c>
-      <c r="E107" t="n">
-        <v>0</v>
-      </c>
-      <c r="F107" t="n">
-        <v>236.76</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>1461</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>ΜΠΑΙΛΑΚΗ ΕΙΡΗΝΗ ΤΟΥ ΜΙΧΑΗΛ</t>
-        </is>
-      </c>
-      <c r="C108" t="n">
-        <v>0</v>
-      </c>
-      <c r="D108" t="n">
-        <v>-29.54</v>
-      </c>
-      <c r="E108" t="n">
-        <v>0</v>
-      </c>
-      <c r="F108" t="n">
-        <v>-29.54</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" t="inlineStr">
-        <is>
-          <t>1444</t>
-        </is>
-      </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>ΠΑΠΑΔΑΚΗ ΕΥΑΓΓΕΛΙΑ &amp; ΣΙΑ ΕΕ</t>
-        </is>
-      </c>
-      <c r="C109" t="n">
-        <v>368.52</v>
-      </c>
-      <c r="D109" t="n">
-        <v>43.49</v>
-      </c>
-      <c r="E109" t="n">
-        <v>0</v>
-      </c>
-      <c r="F109" t="n">
-        <v>412.01</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" t="inlineStr">
-        <is>
-          <t>0173</t>
-        </is>
-      </c>
-      <c r="B110" t="inlineStr">
-        <is>
-          <t>ΠΑΠΑΔΑΚΗ ΕΥΑΓΓΕΛΙΑ</t>
-        </is>
-      </c>
-      <c r="C110" t="n">
-        <v>74.98</v>
-      </c>
-      <c r="D110" t="n">
-        <v>70.67</v>
-      </c>
-      <c r="E110" t="n">
-        <v>25.48</v>
-      </c>
-      <c r="F110" t="n">
-        <v>171.13</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" t="inlineStr">
-        <is>
-          <t>0212</t>
-        </is>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>ΧΑΤΖΙΔΑΚΙ ΕΠΑΜ. ΑΡΓΥΡΗ</t>
-        </is>
-      </c>
-      <c r="C111" t="n">
-        <v>0</v>
-      </c>
-      <c r="D111" t="n">
-        <v>-13.02</v>
-      </c>
-      <c r="E111" t="n">
-        <v>0</v>
-      </c>
-      <c r="F111" t="n">
-        <v>-13.02</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>